<commit_message>
working on adjusting weights based on input
</commit_message>
<xml_diff>
--- a/app/outputs/total_score_from_upload.xlsx
+++ b/app/outputs/total_score_from_upload.xlsx
@@ -235,7 +235,7 @@
     <t>Yum! Brands</t>
   </si>
   <si>
-    <t>402.0</t>
+    <t>214.0</t>
   </si>
 </sst>
 </file>
@@ -1108,8 +1108,8 @@
       <c r="A6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
-        <v>73</v>
+      <c r="B6">
+        <v>103</v>
       </c>
       <c r="C6">
         <v>110</v>
@@ -3027,8 +3027,8 @@
       <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="B25">
-        <v>211</v>
+      <c r="B25" t="s">
+        <v>73</v>
       </c>
       <c r="C25">
         <v>0</v>

</xml_diff>

<commit_message>
fixed single graph output issues
</commit_message>
<xml_diff>
--- a/app/outputs/total_score_from_upload.xlsx
+++ b/app/outputs/total_score_from_upload.xlsx
@@ -235,7 +235,7 @@
     <t>Yum! Brands</t>
   </si>
   <si>
-    <t>214.0</t>
+    <t>216.0</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1109,7 @@
         <v>37</v>
       </c>
       <c r="B6">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6">
         <v>110</v>

</xml_diff>

<commit_message>
added code fix weight updates
</commit_message>
<xml_diff>
--- a/app/outputs/total_score_from_upload.xlsx
+++ b/app/outputs/total_score_from_upload.xlsx
@@ -235,7 +235,7 @@
     <t>Yum! Brands</t>
   </si>
   <si>
-    <t>216.0</t>
+    <t>13234.0</t>
   </si>
 </sst>
 </file>
@@ -3082,7 +3082,7 @@
         <v>104</v>
       </c>
       <c r="T25">
-        <v>411</v>
+        <v>444</v>
       </c>
       <c r="U25">
         <v>111</v>

</xml_diff>

<commit_message>
removed click dependency of weight loading
</commit_message>
<xml_diff>
--- a/app/outputs/total_score_from_upload.xlsx
+++ b/app/outputs/total_score_from_upload.xlsx
@@ -235,7 +235,7 @@
     <t>Yum! Brands</t>
   </si>
   <si>
-    <t>13234.0</t>
+    <t>4813.0</t>
   </si>
 </sst>
 </file>
@@ -3027,8 +3027,8 @@
       <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="B25" t="s">
-        <v>73</v>
+      <c r="B25">
+        <v>442</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -3070,7 +3070,7 @@
         <v>101</v>
       </c>
       <c r="P25">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="Q25">
         <v>110</v>
@@ -3081,8 +3081,8 @@
       <c r="S25">
         <v>104</v>
       </c>
-      <c r="T25">
-        <v>444</v>
+      <c r="T25" t="s">
+        <v>73</v>
       </c>
       <c r="U25">
         <v>111</v>

</xml_diff>

<commit_message>
added partner tracking sheet
</commit_message>
<xml_diff>
--- a/app/outputs/total_score_from_upload.xlsx
+++ b/app/outputs/total_score_from_upload.xlsx
@@ -235,7 +235,7 @@
     <t>Yum! Brands</t>
   </si>
   <si>
-    <t>400.0</t>
+    <t>1.0</t>
   </si>
 </sst>
 </file>
@@ -2630,7 +2630,7 @@
         <v>11</v>
       </c>
       <c r="D21">
-        <v>111</v>
+        <v>311</v>
       </c>
       <c r="E21">
         <v>10</v>
@@ -3735,13 +3735,13 @@
         <v>63</v>
       </c>
       <c r="B32">
-        <v>800</v>
-      </c>
-      <c r="C32" t="s">
+        <v>200</v>
+      </c>
+      <c r="C32">
+        <v>400</v>
+      </c>
+      <c r="D32" t="s">
         <v>73</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
       </c>
       <c r="E32">
         <v>1</v>

</xml_diff>